<commit_message>
Finished adding the infrastructure, now need to implement declining and None requests
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -747,14 +747,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="106" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="5" width="30.7265625" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" customWidth="1"/>
+    <col min="6" max="6" width="17.90625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="18.54296875" customWidth="1"/>
     <col min="9" max="10" width="30.7265625" customWidth="1"/>

</xml_diff>

<commit_message>
Finished the full version of the CCC assigner; now able to queue performers without preference and assign them at the end
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="98" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
planned months now in Excel, and directory was reorganized
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Records" sheetId="1" r:id="rId1"/>
-    <sheet name="School Exceptions" sheetId="2" r:id="rId2"/>
+    <sheet name="Planned Months" sheetId="3" r:id="rId2"/>
+    <sheet name="School Exceptions" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="118">
   <si>
     <t xml:space="preserve">Name: </t>
   </si>
@@ -371,6 +372,9 @@
   </si>
   <si>
     <t>NS</t>
+  </si>
+  <si>
+    <t>Planned Months</t>
   </si>
 </sst>
 </file>
@@ -747,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="98" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView topLeftCell="C1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2484,6 +2488,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>